<commit_message>
Framework, Ebola, User account changes.
</commit_message>
<xml_diff>
--- a/SRFROWCA/TEST/Burkina.xlsx
+++ b/SRFROWCA/TEST/Burkina.xlsx
@@ -457,6 +457,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -467,7 +468,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -775,9 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -798,65 +796,65 @@
     <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -931,236 +929,236 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -1247,236 +1245,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
     </row>
     <row r="15" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">

</xml_diff>